<commit_message>
updated the adt's to different files
</commit_message>
<xml_diff>
--- a/Chess ADT plan.xlsx
+++ b/Chess ADT plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://technionmail-my.sharepoint.com/personal/guycoh_campus_technion_ac_il/Documents/1 Courses/מבוא לתכנות מערכות/HW/HW1/Chess/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="498" documentId="8_{C52EADB1-DC08-054B-BA97-FE992917F3A9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{86F9E424-E21D-A04E-AAC1-975CA3197A38}"/>
+  <xr:revisionPtr revIDLastSave="511" documentId="8_{C52EADB1-DC08-054B-BA97-FE992917F3A9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{B7C320AD-8C48-B142-8A38-168D8C6274FA}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21900" activeTab="1" xr2:uid="{71E549D7-C5B6-1F42-B866-3BBA66337262}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="72">
   <si>
     <t>Chess System</t>
   </si>
@@ -117,15 +117,6 @@
     <t>Version 2</t>
   </si>
   <si>
-    <t>All Players</t>
-  </si>
-  <si>
-    <t>player_statistics_map</t>
-  </si>
-  <si>
-    <t>Player statistics</t>
-  </si>
-  <si>
     <t>Return Values</t>
   </si>
   <si>
@@ -196,9 +187,6 @@
   </si>
   <si>
     <t>Players</t>
-  </si>
-  <si>
-    <t>Player Statistics</t>
   </si>
   <si>
     <t>library</t>
@@ -1047,15 +1035,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>10584</xdr:colOff>
+      <xdr:colOff>42334</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>814917</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>105834</xdr:rowOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>116417</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1070,61 +1058,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="6752167" y="1534583"/>
-          <a:ext cx="1629833" cy="645584"/>
-        </a:xfrm>
-        <a:prstGeom prst="curvedConnector3">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="19050">
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="dk1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>1576917</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="16" name="Curved Connector 15">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{91FBD069-BD38-C541-8A47-7D892DFC3690}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6720417" y="2402417"/>
-          <a:ext cx="1672166" cy="1418166"/>
+          <a:off x="6783917" y="931333"/>
+          <a:ext cx="1598083" cy="21167"/>
         </a:xfrm>
         <a:prstGeom prst="curvedConnector3">
           <a:avLst/>
@@ -1180,6 +1115,59 @@
           <a:ext cx="2286000" cy="1841500"/>
         </a:xfrm>
         <a:prstGeom prst="curvedConnector3">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="19050">
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1587500</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>116417</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>116417</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="22" name="Straight Arrow Connector 21">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4C723073-3B3B-5146-94F4-545703CC479D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6731000" y="1164167"/>
+          <a:ext cx="1661583" cy="1883833"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
           <a:avLst/>
         </a:prstGeom>
         <a:ln w="19050">
@@ -1506,7 +1494,7 @@
   <dimension ref="A2:K108"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1532,8 +1520,8 @@
       </c>
     </row>
     <row r="5" spans="3:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="F5" s="6" t="s">
-        <v>6</v>
+      <c r="F5" s="7" t="s">
+        <v>4</v>
       </c>
       <c r="I5" s="4" t="s">
         <v>3</v>
@@ -1541,7 +1529,7 @@
     </row>
     <row r="6" spans="3:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F6" s="7" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="I6" s="5" t="s">
         <v>11</v>
@@ -1552,7 +1540,7 @@
         <v>0</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="I7" s="6" t="s">
         <v>10</v>
@@ -1563,7 +1551,7 @@
         <v>14</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>4</v>
+        <v>71</v>
       </c>
       <c r="I8" s="8" t="s">
         <v>7</v>
@@ -1574,87 +1562,74 @@
         <v>5</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="F10" s="7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="F11" s="7" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="12" spans="3:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="F12" s="8" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="3:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="F10" s="8" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="3:9" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="14" spans="3:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="I14" s="4" t="s">
-        <v>28</v>
+        <v>49</v>
       </c>
     </row>
     <row r="15" spans="3:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="F15" s="4" t="s">
+        <v>49</v>
+      </c>
       <c r="I15" s="5" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="16" spans="3:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="F16" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="I16" s="6" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="5:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="F17" s="4" t="s">
-        <v>26</v>
+    <row r="17" spans="5:9" x14ac:dyDescent="0.2">
+      <c r="F17" s="6" t="s">
+        <v>18</v>
       </c>
       <c r="I17" s="7" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="5:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="F18" s="5" t="s">
-        <v>12</v>
+    <row r="18" spans="5:9" x14ac:dyDescent="0.2">
+      <c r="F18" s="7" t="s">
+        <v>19</v>
       </c>
       <c r="I18" s="7" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="19" spans="5:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="F19" s="6" t="s">
-        <v>18</v>
+      <c r="F19" s="7" t="s">
+        <v>20</v>
       </c>
       <c r="I19" s="8" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="5:9" x14ac:dyDescent="0.2">
-      <c r="F20" s="7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="21" spans="5:9" x14ac:dyDescent="0.2">
-      <c r="F21" s="7" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="22" spans="5:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="F22" s="8" t="s">
+    <row r="20" spans="5:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="F20" s="8" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="23" spans="5:9" x14ac:dyDescent="0.2">
       <c r="E23" s="3"/>
     </row>
-    <row r="46" spans="9:9" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="47" spans="9:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="6:9" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="47" spans="6:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="F47" s="11"/>
       <c r="I47" s="11"/>
     </row>
-    <row r="48" spans="9:9" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="48" spans="6:9" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="49" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A49" s="10" t="s">
         <v>25</v>
@@ -1663,32 +1638,41 @@
       <c r="C49" s="11"/>
       <c r="D49" s="11"/>
       <c r="E49" s="11"/>
-      <c r="F49" s="11"/>
       <c r="G49" s="11"/>
       <c r="H49" s="11"/>
       <c r="J49" s="11"/>
       <c r="K49" s="12"/>
     </row>
-    <row r="53" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="51" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="52" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="F52" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="F53" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
     <row r="54" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="F54" s="4" t="s">
-        <v>1</v>
+      <c r="F54" s="6" t="s">
+        <v>6</v>
       </c>
       <c r="I54" s="4" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="55" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="F55" s="5" t="s">
-        <v>13</v>
+      <c r="F55" s="7" t="s">
+        <v>8</v>
       </c>
       <c r="I55" s="5" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="F56" s="6" t="s">
-        <v>6</v>
+      <c r="F56" s="7" t="s">
+        <v>9</v>
       </c>
       <c r="I56" s="6" t="s">
         <v>10</v>
@@ -1696,7 +1680,7 @@
     </row>
     <row r="57" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F57" s="7" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="I57" s="7" t="s">
         <v>16</v>
@@ -1707,7 +1691,7 @@
         <v>0</v>
       </c>
       <c r="F58" s="7" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="I58" s="7" t="s">
         <v>15</v>
@@ -1718,7 +1702,7 @@
         <v>14</v>
       </c>
       <c r="F59" s="7" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="I59" s="8" t="s">
         <v>7</v>
@@ -1727,21 +1711,11 @@
     <row r="60" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C60" s="8"/>
       <c r="F60" s="7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="F61" s="7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="F62" s="7" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="63" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="F63" s="8" t="s">
+    <row r="61" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="F61" s="8" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1781,6 +1755,7 @@
     </row>
     <row r="78" spans="5:9" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="79" spans="5:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="F79" s="11"/>
       <c r="I79" s="11"/>
     </row>
     <row r="80" spans="5:9" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
@@ -1792,32 +1767,41 @@
       <c r="C81" s="11"/>
       <c r="D81" s="11"/>
       <c r="E81" s="11"/>
-      <c r="F81" s="11"/>
       <c r="G81" s="11"/>
       <c r="H81" s="11"/>
       <c r="J81" s="11"/>
       <c r="K81" s="12"/>
     </row>
-    <row r="87" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="85" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="86" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="F86" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="F87" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
     <row r="88" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="F88" s="4" t="s">
-        <v>1</v>
+      <c r="F88" s="6" t="s">
+        <v>6</v>
       </c>
       <c r="I88" s="4" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="89" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="F89" s="5" t="s">
-        <v>13</v>
+      <c r="F89" s="7" t="s">
+        <v>8</v>
       </c>
       <c r="I89" s="5" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="90" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="F90" s="6" t="s">
-        <v>6</v>
+      <c r="F90" s="7" t="s">
+        <v>9</v>
       </c>
       <c r="I90" s="6" t="s">
         <v>10</v>
@@ -1825,7 +1809,7 @@
     </row>
     <row r="91" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F91" s="7" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="I91" s="7" t="s">
         <v>16</v>
@@ -1836,7 +1820,7 @@
         <v>0</v>
       </c>
       <c r="F92" s="7" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="I92" s="7" t="s">
         <v>15</v>
@@ -1847,7 +1831,7 @@
         <v>14</v>
       </c>
       <c r="F93" s="7" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="I93" s="8" t="s">
         <v>7</v>
@@ -1858,55 +1842,47 @@
         <v>5</v>
       </c>
       <c r="F94" s="7" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="F95" s="7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="F96" s="7" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="97" spans="5:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="F97" s="8" t="s">
+    <row r="95" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="F95" s="8" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="102" spans="5:6" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="103" spans="5:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="F103" s="4" t="s">
+    <row r="100" spans="5:6" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="101" spans="5:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="F101" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="104" spans="5:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="F104" s="5" t="s">
+    <row r="102" spans="5:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="F102" s="5" t="s">
         <v>12</v>
       </c>
     </row>
+    <row r="103" spans="5:6" x14ac:dyDescent="0.2">
+      <c r="F103" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="104" spans="5:6" x14ac:dyDescent="0.2">
+      <c r="F104" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
     <row r="105" spans="5:6" x14ac:dyDescent="0.2">
-      <c r="F105" s="6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="106" spans="5:6" x14ac:dyDescent="0.2">
-      <c r="F106" s="7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="107" spans="5:6" x14ac:dyDescent="0.2">
-      <c r="F107" s="7" t="s">
+      <c r="F105" s="7" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="108" spans="5:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="5:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="F106" s="8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="108" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E108" s="3"/>
-      <c r="F108" s="8" t="s">
-        <v>21</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1919,7 +1895,7 @@
   <dimension ref="A2:K25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1940,7 +1916,7 @@
     <row r="2" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>0</v>
@@ -1952,7 +1928,7 @@
         <v>3</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -1984,7 +1960,7 @@
       </c>
     </row>
     <row r="6" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="E6" s="8" t="s">
+      <c r="E6" s="7" t="s">
         <v>5</v>
       </c>
       <c r="G6" s="8" t="s">
@@ -2004,7 +1980,7 @@
     </row>
     <row r="8" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="E8" s="7" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="I8" s="8" t="s">
         <v>21</v>
@@ -2037,10 +2013,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A26AF13F-382D-EE4D-8DB2-01DAED232B99}">
-  <dimension ref="A1:F34"/>
+  <dimension ref="A1:E34"/>
   <sheetViews>
     <sheetView zoomScale="133" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2050,13 +2026,12 @@
     <col min="3" max="3" width="30.83203125" style="1" customWidth="1"/>
     <col min="4" max="4" width="23.33203125" style="1" customWidth="1"/>
     <col min="5" max="5" width="27.1640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="17.6640625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="35" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="35" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="22" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B1" s="23" t="s">
         <v>0</v>
@@ -2070,317 +2045,281 @@
       <c r="E1" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="23" t="s">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" s="29" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" s="29" t="s">
+        <v>66</v>
+      </c>
+      <c r="D2" s="29" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="24" t="s">
-        <v>55</v>
-      </c>
-      <c r="B2" s="29" t="s">
-        <v>49</v>
-      </c>
-      <c r="C2" s="29" t="s">
-        <v>70</v>
-      </c>
-      <c r="D2" s="29" t="s">
-        <v>57</v>
-      </c>
       <c r="E2" s="29" t="s">
-        <v>60</v>
-      </c>
-      <c r="F2" s="29"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="25"/>
       <c r="B3" s="30" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C3" s="30" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="D3" s="30" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="E3" s="30" t="s">
-        <v>61</v>
-      </c>
-      <c r="F3" s="30"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="25"/>
       <c r="B4" s="30" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C4" s="30"/>
       <c r="D4" s="30" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="E4" s="30" t="s">
-        <v>58</v>
-      </c>
-      <c r="F4" s="30"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="25"/>
       <c r="B5" s="30" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C5" s="30"/>
       <c r="D5" s="30" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="E5" s="30" t="s">
-        <v>72</v>
-      </c>
-      <c r="F5" s="30"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="25"/>
       <c r="B6" s="30" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C6" s="30"/>
       <c r="D6" s="30"/>
       <c r="E6" s="30" t="s">
-        <v>62</v>
-      </c>
-      <c r="F6" s="30"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="25"/>
       <c r="B7" s="30" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C7" s="30"/>
       <c r="D7" s="30"/>
       <c r="E7" s="30"/>
-      <c r="F7" s="30"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="25"/>
       <c r="B8" s="30" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C8" s="30"/>
       <c r="D8" s="30"/>
       <c r="E8" s="30"/>
-      <c r="F8" s="30"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="25"/>
       <c r="B9" s="30" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C9" s="30"/>
       <c r="D9" s="30"/>
       <c r="E9" s="30"/>
-      <c r="F9" s="30"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="25"/>
       <c r="B10" s="30" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C10" s="30"/>
       <c r="D10" s="30"/>
       <c r="E10" s="30"/>
-      <c r="F10" s="30"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="25"/>
       <c r="B11" s="30" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C11" s="30"/>
       <c r="D11" s="30"/>
       <c r="E11" s="30"/>
-      <c r="F11" s="30"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="25"/>
       <c r="B12" s="30"/>
       <c r="C12" s="30"/>
       <c r="D12" s="30"/>
       <c r="E12" s="30"/>
-      <c r="F12" s="30"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="25"/>
       <c r="B13" s="30"/>
       <c r="C13" s="30"/>
       <c r="D13" s="30"/>
       <c r="E13" s="30"/>
-      <c r="F13" s="30"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="26"/>
       <c r="B14" s="30"/>
       <c r="C14" s="30"/>
       <c r="D14" s="30"/>
       <c r="E14" s="30"/>
-      <c r="F14" s="30"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="27"/>
       <c r="B15" s="30"/>
       <c r="C15" s="30"/>
       <c r="D15" s="30"/>
       <c r="E15" s="30"/>
-      <c r="F15" s="30"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="27"/>
       <c r="B16" s="30"/>
       <c r="C16" s="30"/>
       <c r="D16" s="30"/>
       <c r="E16" s="30"/>
-      <c r="F16" s="30"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="27"/>
       <c r="B17" s="30"/>
       <c r="C17" s="30"/>
       <c r="D17" s="30"/>
       <c r="E17" s="30"/>
-      <c r="F17" s="30"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="27"/>
       <c r="B18" s="30"/>
       <c r="C18" s="30"/>
       <c r="D18" s="30"/>
       <c r="E18" s="30"/>
-      <c r="F18" s="30"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="27"/>
       <c r="B19" s="30"/>
       <c r="C19" s="30"/>
       <c r="D19" s="30"/>
       <c r="E19" s="30"/>
-      <c r="F19" s="30"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="27"/>
       <c r="B20" s="30"/>
       <c r="C20" s="30"/>
       <c r="D20" s="30"/>
       <c r="E20" s="30"/>
-      <c r="F20" s="30"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="27"/>
       <c r="B21" s="30"/>
       <c r="C21" s="30"/>
       <c r="D21" s="30"/>
       <c r="E21" s="30"/>
-      <c r="F21" s="30"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="27"/>
       <c r="B22" s="30"/>
       <c r="C22" s="30"/>
       <c r="D22" s="30"/>
       <c r="E22" s="30"/>
-      <c r="F22" s="30"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="27"/>
       <c r="B23" s="30"/>
       <c r="C23" s="30"/>
       <c r="D23" s="30"/>
       <c r="E23" s="30"/>
-      <c r="F23" s="30"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="27"/>
       <c r="B24" s="7"/>
       <c r="C24" s="7"/>
       <c r="D24" s="7"/>
       <c r="E24" s="7"/>
-      <c r="F24" s="7"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="27"/>
       <c r="B25" s="7"/>
       <c r="C25" s="7"/>
       <c r="D25" s="7"/>
       <c r="E25" s="7"/>
-      <c r="F25" s="7"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="27"/>
       <c r="B26" s="7"/>
       <c r="C26" s="7"/>
       <c r="D26" s="7"/>
       <c r="E26" s="7"/>
-      <c r="F26" s="7"/>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="27"/>
       <c r="B27" s="7"/>
       <c r="C27" s="7"/>
       <c r="D27" s="7"/>
       <c r="E27" s="7"/>
-      <c r="F27" s="7"/>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="27"/>
       <c r="B28" s="7"/>
       <c r="C28" s="7"/>
       <c r="D28" s="7"/>
       <c r="E28" s="7"/>
-      <c r="F28" s="7"/>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="27"/>
       <c r="B29" s="7"/>
       <c r="C29" s="7"/>
       <c r="D29" s="7"/>
       <c r="E29" s="7"/>
-      <c r="F29" s="7"/>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="27"/>
       <c r="B30" s="7"/>
       <c r="C30" s="7"/>
       <c r="D30" s="7"/>
       <c r="E30" s="7"/>
-      <c r="F30" s="7"/>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="27"/>
       <c r="B31" s="7"/>
       <c r="C31" s="7"/>
       <c r="D31" s="7"/>
       <c r="E31" s="7"/>
-      <c r="F31" s="7"/>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="27"/>
       <c r="B32" s="7"/>
       <c r="C32" s="7"/>
       <c r="D32" s="7"/>
       <c r="E32" s="7"/>
-      <c r="F32" s="7"/>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="27"/>
       <c r="B33" s="7"/>
       <c r="C33" s="7"/>
       <c r="D33" s="7"/>
       <c r="E33" s="7"/>
-      <c r="F33" s="7"/>
-    </row>
-    <row r="34" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="28"/>
       <c r="B34" s="8"/>
       <c r="C34" s="8"/>
       <c r="D34" s="8"/>
       <c r="E34" s="8"/>
-      <c r="F34" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2408,113 +2347,113 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="34" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="20" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B2" s="21"/>
     </row>
     <row r="3" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" s="18" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="19" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B4" s="14"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="19" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B5" s="14"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="19" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B6" s="14"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="19" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B7" s="14"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="19" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B8" s="14"/>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="19" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B9" s="14"/>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="19" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B10" s="14"/>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="19" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B11" s="14"/>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="19" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B12" s="14"/>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="19" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B13" s="14"/>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="19" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B14" s="14"/>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="19" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B15" s="14"/>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="19" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B16" s="14"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="19" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B17" s="14"/>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="19" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B18" s="14"/>
     </row>

</xml_diff>